<commit_message>
new wifi lan classes
</commit_message>
<xml_diff>
--- a/en2.xlsx
+++ b/en2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_mesDocs\_git\ts-tool-assets\locales\en-GB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_mesDocs\_git\trouble_shooting\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,32 +14,32 @@
   <sheets>
     <sheet name="Validators" sheetId="13" r:id="rId1"/>
     <sheet name="Meta" sheetId="12" r:id="rId2"/>
-    <sheet name="WiFi_LAN" sheetId="11" r:id="rId3"/>
-    <sheet name="Stability" sheetId="10" r:id="rId4"/>
+    <sheet name="wifi-lan_en" sheetId="11" r:id="rId3"/>
+    <sheet name="stability_en" sheetId="10" r:id="rId4"/>
     <sheet name="tv" sheetId="9" r:id="rId5"/>
-    <sheet name="NoInternet" sheetId="8" r:id="rId6"/>
-    <sheet name="instalation_activation" sheetId="7" r:id="rId7"/>
+    <sheet name="nointernet_en" sheetId="8" r:id="rId6"/>
+    <sheet name="installation-activation_en" sheetId="7" r:id="rId7"/>
     <sheet name="Escalation" sheetId="6" r:id="rId8"/>
     <sheet name="equipment" sheetId="5" r:id="rId9"/>
     <sheet name="collection" sheetId="4" r:id="rId10"/>
-    <sheet name="cables" sheetId="3" r:id="rId11"/>
+    <sheet name="cables_en" sheetId="3" r:id="rId11"/>
     <sheet name="all" sheetId="2" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="all_en" localSheetId="11">all!$A$1:$H$14</definedName>
-    <definedName name="cables_en" localSheetId="10">cables!$A$1:$H$10</definedName>
+    <definedName name="cables_en" localSheetId="10">cables_en!$A$1:$H$10</definedName>
     <definedName name="collection_en" localSheetId="9">collection!$A$1:$H$17</definedName>
     <definedName name="equipment_en" localSheetId="8">equipment!$A$1:$H$24</definedName>
     <definedName name="escalation_en" localSheetId="7">Escalation!$A$1:$H$18</definedName>
-    <definedName name="installation_activation_en" localSheetId="6">instalation_activation!$A$1:$H$15</definedName>
+    <definedName name="installation_activation_en" localSheetId="6">'installation-activation_en'!$A$1:$H$15</definedName>
     <definedName name="meta_en" localSheetId="1">Meta!$A$1:$D$9</definedName>
-    <definedName name="nointernet_en" localSheetId="5">NoInternet!$A$1:$H$34</definedName>
+    <definedName name="nointernet_en" localSheetId="5">nointernet_en!$A$1:$H$34</definedName>
     <definedName name="salttv_en" localSheetId="4">tv!$A$1:$H$28</definedName>
-    <definedName name="stability_en" localSheetId="3">Stability!$A$1:$H$20</definedName>
+    <definedName name="stability_en" localSheetId="3">stability_en!$A$1:$H$20</definedName>
     <definedName name="validator_en" localSheetId="0">Validators!$A$1:$F$4</definedName>
-    <definedName name="wifi_lan_en" localSheetId="2">WiFi_LAN!$A$1:$H$28</definedName>
+    <definedName name="wifi_lan_en" localSheetId="2">'wifi-lan_en'!$A$1:$H$28</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -216,7 +216,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="777">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="782">
   <si>
     <t>FLAG</t>
   </si>
@@ -559,9 +559,6 @@
     <t>A ticket [321] will be automatically generated upon advancing to the next step. Do not manually create one (SuperOffice). A copy of the content will be sent to your mailbox.&lt;N&gt;&lt;N&gt;DON'T PROMISE ANYTHING!</t>
   </si>
   <si>
-    <t>Automatic ticket creation [321] in SuperOffice</t>
-  </si>
-  <si>
     <t>so/compensationen</t>
   </si>
   <si>
@@ -736,9 +733,6 @@
     <t>$flow.equipment._ParcelIsBackToSalt</t>
   </si>
   <si>
-    <t>Inform that the package has been returned to us.</t>
-  </si>
-  <si>
     <t>$flow.equipment._ResendValidationEmail</t>
   </si>
   <si>
@@ -961,9 +955,6 @@
     <t>He will be contacted within 48 hours&lt;N&gt;&lt;N&gt;&lt;N&gt;Ask if:&lt;N&gt;&lt;T&gt;- the contact information (mobile number, e-mail address) is correct,&lt;N&gt;&lt;T&gt;- the customer prefers to be contacted by phone, SMS, e-mail, WhatsApp or another channel. &lt;N&gt;&lt;N&gt;Inform that:&lt;N&gt;&lt;T&gt;- a technical ticket is forwarded to our technical department for a thorough analysis.&lt;N&gt;&lt;T&gt;- he may be contacted.&lt;N&gt;&lt;T&gt;- he will receive feedback as soon as possible.&lt;N&gt;&lt;T&gt; - the box must always be powered (230V) and plugged in (SFP, Fibre, OTO) during the whole life of a ticket.</t>
   </si>
   <si>
-    <t>Inform the customer that the ticket will be treated with priority</t>
-  </si>
-  <si>
     <t>$flow.escalation._SolveCustomerIssue</t>
   </si>
   <si>
@@ -1147,9 +1138,6 @@
     <t>If the box is plugged into a multiplug, plug directly into the wall socket. &lt;N&gt;Try another wall socket.</t>
   </si>
   <si>
-    <t>Check the connections of the electrical socket</t>
-  </si>
-  <si>
     <t>$flow.activation._SendCustomerBAckToStore</t>
   </si>
   <si>
@@ -1297,9 +1285,6 @@
     <t>&lt;T&gt; - Correct OTO number on the socket&lt;N&gt;&lt;T&gt; - Correct OTO port number used&lt;N&gt;&lt;T&gt; - Fiber cable connected with the blue lever looking up&lt;N&gt;&lt;T&gt; - Power cable connected</t>
   </si>
   <si>
-    <t>Is the installation OK?</t>
-  </si>
-  <si>
     <t>box/blueleverup</t>
   </si>
   <si>
@@ -1735,9 +1720,6 @@
     <t>Ask the customer to verify on the back of the router.</t>
   </si>
   <si>
-    <t>Make sure the Apple TV is connected to the 1Ghz ethernet port</t>
-  </si>
-  <si>
     <t>box/lan/lan</t>
   </si>
   <si>
@@ -2042,9 +2024,6 @@
   </si>
   <si>
     <t>$flow.stability._AtWhatTimeDoesItOccurs</t>
-  </si>
-  <si>
-    <t>In what time slot does this happen?</t>
   </si>
   <si>
     <t>$flow.stability._WhenDidItStart</t>
@@ -2279,9 +2258,6 @@
     <t>(not directly to the box)</t>
   </si>
   <si>
-    <t>The device is connected through a switch</t>
-  </si>
-  <si>
     <t>$flow.lan.LanConnectionOK</t>
   </si>
   <si>
@@ -2378,9 +2354,6 @@
     <t>$flow.wifi.WifiOnInDashboard</t>
   </si>
   <si>
-    <t>Are the 2 WiFi are green in the dashboard?</t>
-  </si>
-  <si>
     <t>vti/WifiOnInDashboard-en</t>
   </si>
   <si>
@@ -2471,9 +2444,6 @@
     <t>Try with another device in LAN</t>
   </si>
   <si>
-    <t>All explained</t>
-  </si>
-  <si>
     <t>flag</t>
   </si>
   <si>
@@ -2550,6 +2520,51 @@
   </si>
   <si>
     <t>(Valeur RX)</t>
+  </si>
+  <si>
+    <t>Reboot DONE</t>
+  </si>
+  <si>
+    <t>Could not reboot</t>
+  </si>
+  <si>
+    <t>Are the 2 WiFi green in the dashboard?</t>
+  </si>
+  <si>
+    <t>$flow.wifi._CanSeeGoogle</t>
+  </si>
+  <si>
+    <t>Could see Google</t>
+  </si>
+  <si>
+    <t>no connection at all</t>
+  </si>
+  <si>
+    <t>Test Google and then other on the device's browser</t>
+  </si>
+  <si>
+    <t>Can see google but not another</t>
+  </si>
+  <si>
+    <t>Have the customer openening a browser and enter google.com&lt;N&gt;If he can reach it than no ticket will be created &lt;b&gt;unless you state the url or app&lt;b&gt; that still doesn't work.</t>
+  </si>
+  <si>
+    <t>$flow.lan.OkToTryWifi</t>
+  </si>
+  <si>
+    <t>Now let's try to see if it work on WiFi</t>
+  </si>
+  <si>
+    <t>Ok let's go</t>
+  </si>
+  <si>
+    <t>No, cannot do</t>
+  </si>
+  <si>
+    <t>In the majority of cases customer have WiFi devices and it will be very insightful to try.&lt;N&gt;In other cases either the customer has no WiFi device or he asserts it isworking fine with WiFi, select NO then a LAN ISSUE ticket will be created.</t>
+  </si>
+  <si>
+    <t>The device is connected through a switch ?</t>
   </si>
 </sst>
 </file>
@@ -2607,7 +2622,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2624,6 +2639,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2971,46 +2992,46 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>751</v>
+        <v>741</v>
       </c>
       <c r="B1" t="s">
-        <v>771</v>
+        <v>761</v>
       </c>
       <c r="C1" t="s">
-        <v>772</v>
+        <v>762</v>
       </c>
       <c r="D1" t="s">
-        <v>773</v>
+        <v>763</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="B2" t="s">
-        <v>774</v>
+        <v>764</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="B3" t="s">
-        <v>775</v>
+        <v>765</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="B4" t="s">
-        <v>776</v>
+        <v>766</v>
       </c>
       <c r="C4" t="s">
-        <v>776</v>
+        <v>766</v>
       </c>
       <c r="D4" t="s">
-        <v>776</v>
+        <v>766</v>
       </c>
     </row>
   </sheetData>
@@ -3022,7 +3043,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3128,147 +3151,147 @@
         <v>112</v>
       </c>
       <c r="C7" t="s">
+        <v>781</v>
+      </c>
+      <c r="D7" t="s">
         <v>113</v>
-      </c>
-      <c r="D7" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" t="s">
         <v>115</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>116</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>117</v>
       </c>
-      <c r="D8" t="s">
+      <c r="H8" t="s">
         <v>118</v>
-      </c>
-      <c r="H8" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" t="s">
         <v>120</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>121</v>
-      </c>
-      <c r="C9" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" t="s">
         <v>123</v>
-      </c>
-      <c r="C10" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B11" t="s">
         <v>125</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>126</v>
       </c>
-      <c r="C11" t="s">
+      <c r="E11" t="s">
         <v>127</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>128</v>
-      </c>
-      <c r="F11" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>129</v>
+      </c>
+      <c r="C12" t="s">
         <v>130</v>
       </c>
-      <c r="C12" t="s">
+      <c r="E12" t="s">
         <v>131</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>132</v>
-      </c>
-      <c r="F12" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>133</v>
+      </c>
+      <c r="B13" t="s">
         <v>134</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>135</v>
       </c>
-      <c r="C13" t="s">
+      <c r="E13" t="s">
         <v>136</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>137</v>
-      </c>
-      <c r="F13" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" t="s">
         <v>139</v>
       </c>
-      <c r="C14" t="s">
+      <c r="E14" t="s">
         <v>140</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>141</v>
-      </c>
-      <c r="F14" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>142</v>
+      </c>
+      <c r="B15" t="s">
         <v>143</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>144</v>
       </c>
-      <c r="C15" t="s">
+      <c r="H15" t="s">
         <v>145</v>
-      </c>
-      <c r="H15" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>146</v>
+      </c>
+      <c r="B16" t="s">
         <v>147</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>148</v>
       </c>
-      <c r="C16" t="s">
+      <c r="E16" t="s">
         <v>149</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>150</v>
-      </c>
-      <c r="F16" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>151</v>
+      </c>
+      <c r="C17" t="s">
         <v>152</v>
-      </c>
-      <c r="C17" t="s">
-        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -3460,8 +3483,8 @@
   </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3722,89 +3745,89 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>751</v>
+        <v>741</v>
       </c>
       <c r="B1" t="s">
-        <v>752</v>
+        <v>742</v>
       </c>
       <c r="C1" t="s">
-        <v>753</v>
+        <v>743</v>
       </c>
       <c r="D1" t="s">
-        <v>754</v>
+        <v>744</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>755</v>
+        <v>745</v>
       </c>
       <c r="B2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C2" t="s">
-        <v>756</v>
+        <v>746</v>
       </c>
       <c r="D2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="B3" t="s">
-        <v>757</v>
+        <v>747</v>
       </c>
       <c r="C3" t="s">
-        <v>758</v>
+        <v>748</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>759</v>
+        <v>749</v>
       </c>
       <c r="B4" t="s">
-        <v>760</v>
+        <v>750</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>761</v>
+        <v>751</v>
       </c>
       <c r="B5" t="s">
-        <v>762</v>
+        <v>752</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>763</v>
+        <v>753</v>
       </c>
       <c r="B6" t="s">
-        <v>764</v>
+        <v>754</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>765</v>
+        <v>755</v>
       </c>
       <c r="B7" t="s">
-        <v>766</v>
+        <v>756</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>767</v>
+        <v>757</v>
       </c>
       <c r="B8" t="s">
-        <v>768</v>
+        <v>758</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>769</v>
+        <v>759</v>
       </c>
       <c r="B9" t="s">
-        <v>770</v>
+        <v>760</v>
       </c>
     </row>
   </sheetData>
@@ -3815,18 +3838,18 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor rgb="FFFFC000"/>
+    <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="81.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="81.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="72.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.42578125" bestFit="1" customWidth="1"/>
@@ -3839,7 +3862,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -3861,315 +3884,348 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>670</v>
-      </c>
-      <c r="B2" t="s">
-        <v>671</v>
+        <v>663</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>664</v>
       </c>
       <c r="C2" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>672</v>
-      </c>
-      <c r="B3" t="s">
-        <v>673</v>
+        <v>665</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>666</v>
       </c>
       <c r="C3" t="s">
-        <v>674</v>
+        <v>667</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>675</v>
-      </c>
-      <c r="B4" t="s">
-        <v>673</v>
+        <v>668</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>666</v>
       </c>
       <c r="C4" t="s">
-        <v>676</v>
+        <v>669</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>677</v>
-      </c>
-      <c r="B5" t="s">
-        <v>678</v>
+        <v>670</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>671</v>
       </c>
       <c r="C5" t="s">
-        <v>679</v>
+        <v>672</v>
       </c>
       <c r="E5" t="s">
-        <v>680</v>
+        <v>673</v>
       </c>
       <c r="F5" t="s">
-        <v>681</v>
+        <v>674</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>682</v>
+        <v>675</v>
       </c>
       <c r="C6" t="s">
-        <v>683</v>
+        <v>676</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>684</v>
-      </c>
-      <c r="B7" t="s">
-        <v>685</v>
+        <v>677</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>678</v>
       </c>
       <c r="C7" t="s">
-        <v>686</v>
+        <v>781</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>687</v>
+        <v>679</v>
       </c>
       <c r="C8" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>689</v>
-      </c>
-      <c r="B9" t="s">
-        <v>690</v>
+        <v>681</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>682</v>
       </c>
       <c r="C9" t="s">
-        <v>691</v>
+        <v>683</v>
       </c>
       <c r="D9" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>684</v>
+      </c>
+      <c r="C10" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>686</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>687</v>
+      </c>
+      <c r="C11" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>689</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>690</v>
+      </c>
+      <c r="C12" t="s">
+        <v>691</v>
+      </c>
+      <c r="H12" t="s">
         <v>692</v>
-      </c>
-      <c r="C10" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>694</v>
-      </c>
-      <c r="B11" t="s">
-        <v>695</v>
-      </c>
-      <c r="C11" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>697</v>
-      </c>
-      <c r="B12" t="s">
-        <v>698</v>
-      </c>
-      <c r="C12" t="s">
-        <v>699</v>
-      </c>
-      <c r="H12" t="s">
-        <v>700</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>701</v>
+        <v>693</v>
       </c>
       <c r="C13" t="s">
-        <v>702</v>
+        <v>694</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>703</v>
-      </c>
-      <c r="B14" t="s">
-        <v>704</v>
+        <v>695</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>696</v>
       </c>
       <c r="C14" t="s">
-        <v>705</v>
+        <v>697</v>
       </c>
       <c r="D14" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>707</v>
-      </c>
-      <c r="B15" t="s">
-        <v>708</v>
+        <v>699</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>700</v>
       </c>
       <c r="C15" t="s">
-        <v>709</v>
+        <v>701</v>
       </c>
       <c r="H15" t="s">
-        <v>710</v>
+        <v>702</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>711</v>
+        <v>703</v>
       </c>
       <c r="C16" t="s">
-        <v>712</v>
+        <v>704</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>713</v>
+        <v>705</v>
       </c>
       <c r="C17" t="s">
-        <v>714</v>
+        <v>706</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>715</v>
-      </c>
-      <c r="B18" t="s">
-        <v>716</v>
+        <v>707</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>708</v>
       </c>
       <c r="C18" t="s">
-        <v>717</v>
+        <v>709</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>718</v>
+        <v>710</v>
       </c>
       <c r="C19" t="s">
-        <v>719</v>
+        <v>769</v>
       </c>
       <c r="D19" t="s">
-        <v>720</v>
+        <v>711</v>
       </c>
       <c r="H19" t="s">
-        <v>721</v>
+        <v>712</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>722</v>
+        <v>713</v>
       </c>
       <c r="C20" t="s">
-        <v>723</v>
+        <v>714</v>
       </c>
       <c r="H20" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>725</v>
-      </c>
-      <c r="B21" t="s">
-        <v>726</v>
+        <v>716</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>717</v>
       </c>
       <c r="C21" t="s">
-        <v>727</v>
+        <v>718</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>728</v>
+        <v>719</v>
       </c>
       <c r="C22" t="s">
-        <v>729</v>
+        <v>720</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>730</v>
-      </c>
+        <v>721</v>
+      </c>
+      <c r="B23" s="9"/>
       <c r="C23" s="4" t="s">
-        <v>731</v>
+        <v>722</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>732</v>
+        <v>723</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>733</v>
+        <v>724</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>734</v>
+        <v>725</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>735</v>
+        <v>726</v>
       </c>
       <c r="C24" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>737</v>
-      </c>
-      <c r="B25" t="s">
-        <v>738</v>
+        <v>728</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>729</v>
       </c>
       <c r="C25" t="s">
-        <v>739</v>
+        <v>730</v>
       </c>
       <c r="H25" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>741</v>
-      </c>
-      <c r="B26" t="s">
-        <v>742</v>
+        <v>732</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>733</v>
       </c>
       <c r="C26" t="s">
-        <v>743</v>
+        <v>734</v>
       </c>
       <c r="H26" t="s">
-        <v>740</v>
+        <v>731</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>744</v>
+        <v>735</v>
       </c>
       <c r="C27" t="s">
-        <v>745</v>
+        <v>736</v>
       </c>
       <c r="E27" t="s">
-        <v>746</v>
+        <v>737</v>
       </c>
       <c r="F27" t="s">
-        <v>747</v>
+        <v>738</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>748</v>
+        <v>739</v>
       </c>
       <c r="C28" t="s">
-        <v>749</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G29" t="s">
-        <v>750</v>
+        <v>740</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>770</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>775</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>773</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>771</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>772</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>776</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>780</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>777</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>778</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>779</v>
       </c>
     </row>
   </sheetData>
@@ -4185,8 +4241,8 @@
   </sheetPr>
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4229,280 +4285,280 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>592</v>
+        <v>586</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>593</v>
+        <v>587</v>
       </c>
       <c r="C3" t="s">
-        <v>594</v>
+        <v>588</v>
       </c>
       <c r="E3" t="s">
-        <v>595</v>
+        <v>589</v>
       </c>
       <c r="F3" t="s">
-        <v>596</v>
+        <v>590</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
       <c r="B4" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
       <c r="C4" t="s">
-        <v>599</v>
+        <v>593</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>600</v>
+        <v>594</v>
       </c>
       <c r="C5" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
       <c r="C6" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="E6" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="F6" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="G6" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="C7" t="s">
-        <v>608</v>
+        <v>781</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>609</v>
+        <v>602</v>
       </c>
       <c r="C8" t="s">
-        <v>610</v>
+        <v>603</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>611</v>
+        <v>604</v>
       </c>
       <c r="C9" t="s">
-        <v>612</v>
+        <v>605</v>
       </c>
       <c r="E9" t="s">
-        <v>613</v>
+        <v>606</v>
       </c>
       <c r="F9" t="s">
-        <v>614</v>
+        <v>607</v>
       </c>
       <c r="G9" t="s">
-        <v>615</v>
+        <v>608</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>616</v>
+        <v>609</v>
       </c>
       <c r="B10" t="s">
-        <v>617</v>
+        <v>610</v>
       </c>
       <c r="C10" t="s">
-        <v>618</v>
+        <v>611</v>
       </c>
       <c r="H10" t="s">
-        <v>619</v>
+        <v>612</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>620</v>
+        <v>613</v>
       </c>
       <c r="B11" t="s">
-        <v>621</v>
+        <v>614</v>
       </c>
       <c r="C11" t="s">
-        <v>622</v>
+        <v>615</v>
       </c>
       <c r="H11" t="s">
-        <v>623</v>
+        <v>616</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>624</v>
+        <v>617</v>
       </c>
       <c r="B12" t="s">
-        <v>625</v>
+        <v>618</v>
       </c>
       <c r="C12" t="s">
-        <v>626</v>
+        <v>619</v>
       </c>
       <c r="H12" t="s">
-        <v>627</v>
+        <v>620</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>628</v>
+        <v>621</v>
       </c>
       <c r="B13" t="s">
-        <v>629</v>
+        <v>622</v>
       </c>
       <c r="C13" t="s">
-        <v>630</v>
+        <v>623</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>631</v>
+        <v>624</v>
       </c>
       <c r="B14" t="s">
-        <v>632</v>
+        <v>625</v>
       </c>
       <c r="C14" t="s">
-        <v>633</v>
+        <v>626</v>
       </c>
       <c r="D14" t="s">
-        <v>634</v>
+        <v>627</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>635</v>
+        <v>628</v>
       </c>
       <c r="B15" t="s">
-        <v>636</v>
+        <v>629</v>
       </c>
       <c r="C15" t="s">
-        <v>637</v>
+        <v>630</v>
       </c>
       <c r="E15" t="s">
-        <v>638</v>
+        <v>631</v>
       </c>
       <c r="F15" t="s">
-        <v>639</v>
+        <v>632</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>640</v>
+        <v>633</v>
       </c>
       <c r="B16" t="s">
-        <v>641</v>
+        <v>634</v>
       </c>
       <c r="C16" t="s">
-        <v>642</v>
+        <v>635</v>
       </c>
       <c r="E16" t="s">
-        <v>643</v>
+        <v>636</v>
       </c>
       <c r="F16" t="s">
-        <v>644</v>
+        <v>637</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>645</v>
+        <v>638</v>
       </c>
       <c r="B17" t="s">
-        <v>646</v>
+        <v>639</v>
       </c>
       <c r="C17" t="s">
-        <v>647</v>
+        <v>640</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>648</v>
+        <v>641</v>
       </c>
       <c r="C18" t="s">
-        <v>649</v>
+        <v>642</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>650</v>
+        <v>643</v>
       </c>
       <c r="B19" t="s">
-        <v>651</v>
+        <v>644</v>
       </c>
       <c r="C19" t="s">
-        <v>652</v>
+        <v>645</v>
       </c>
       <c r="E19" t="s">
-        <v>653</v>
+        <v>646</v>
       </c>
       <c r="F19" t="s">
-        <v>654</v>
+        <v>647</v>
       </c>
       <c r="G19" t="s">
-        <v>655</v>
+        <v>648</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>656</v>
+        <v>649</v>
       </c>
       <c r="B20" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
       <c r="C20" t="s">
-        <v>658</v>
+        <v>651</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>659</v>
+        <v>652</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>660</v>
+        <v>653</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>661</v>
+        <v>654</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>662</v>
+        <v>655</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>663</v>
+        <v>656</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>664</v>
+        <v>657</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>665</v>
+        <v>658</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>666</v>
+        <v>659</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>667</v>
+        <v>660</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>668</v>
+        <v>661</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>669</v>
+        <v>662</v>
       </c>
     </row>
   </sheetData>
@@ -4514,8 +4570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4558,428 +4614,428 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>471</v>
+      </c>
+      <c r="B2" t="s">
+        <v>472</v>
+      </c>
+      <c r="C2" t="s">
+        <v>473</v>
+      </c>
+      <c r="D2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E2" t="s">
+        <v>475</v>
+      </c>
+      <c r="H2" t="s">
         <v>476</v>
-      </c>
-      <c r="B2" t="s">
-        <v>477</v>
-      </c>
-      <c r="C2" t="s">
-        <v>478</v>
-      </c>
-      <c r="D2" t="s">
-        <v>479</v>
-      </c>
-      <c r="E2" t="s">
-        <v>480</v>
-      </c>
-      <c r="H2" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>477</v>
+      </c>
+      <c r="B3" t="s">
+        <v>478</v>
+      </c>
+      <c r="C3" t="s">
+        <v>479</v>
+      </c>
+      <c r="D3" t="s">
+        <v>480</v>
+      </c>
+      <c r="E3" t="s">
+        <v>481</v>
+      </c>
+      <c r="H3" t="s">
         <v>482</v>
-      </c>
-      <c r="B3" t="s">
-        <v>483</v>
-      </c>
-      <c r="C3" t="s">
-        <v>484</v>
-      </c>
-      <c r="D3" t="s">
-        <v>485</v>
-      </c>
-      <c r="E3" t="s">
-        <v>486</v>
-      </c>
-      <c r="H3" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="B4" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="C4" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="E4" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="H4" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="B5" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="C5" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="D5" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="E5" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="H5" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="B6" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="C6" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="E6" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="H6" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="B7" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="C7" t="s">
-        <v>505</v>
+        <v>781</v>
       </c>
       <c r="D7" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="E7" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>508</v>
+        <v>502</v>
       </c>
       <c r="B8" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="C8" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="B9" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="C9" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="B10" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="C10" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="H10" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="B11" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="C11" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="H11" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="B12" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="C12" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="D12" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="E12" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="B13" t="s">
-        <v>528</v>
+        <v>522</v>
       </c>
       <c r="C13" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="H13" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="B14" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="C14" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="H14" t="s">
-        <v>534</v>
+        <v>528</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="B15" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="C15" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="H15" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="B16" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
       <c r="C16" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
       <c r="H16" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="B17" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
       <c r="C17" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
       <c r="E17" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
       <c r="F17" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
       <c r="B18" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
       <c r="C18" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="D18" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="E18" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
       <c r="F18" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>554</v>
+        <v>548</v>
       </c>
       <c r="B19" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
       <c r="C19" t="s">
-        <v>556</v>
+        <v>550</v>
       </c>
       <c r="D19" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="E19" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="F19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="B20" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="C20" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="E20" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F20" t="s">
-        <v>562</v>
+        <v>556</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
       <c r="C21" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="D21" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
       <c r="E21" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
       <c r="F21" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>566</v>
+        <v>560</v>
       </c>
       <c r="B22" t="s">
-        <v>567</v>
+        <v>561</v>
       </c>
       <c r="C22" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
       <c r="D22" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
       <c r="E22" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="F22" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>571</v>
+        <v>565</v>
       </c>
       <c r="B23" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
       <c r="C23" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
       <c r="E23" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
       <c r="F23" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
       <c r="B24" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="C24" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="E24" t="s">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="F24" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>580</v>
+        <v>574</v>
       </c>
       <c r="B25" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
       <c r="C25" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
       <c r="D25" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="E25" t="s">
-        <v>584</v>
+        <v>578</v>
       </c>
       <c r="F25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H25" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>586</v>
+        <v>580</v>
       </c>
       <c r="C26" t="s">
-        <v>587</v>
+        <v>581</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>588</v>
+        <v>582</v>
       </c>
       <c r="C27" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>590</v>
+        <v>584</v>
       </c>
       <c r="C28" t="s">
-        <v>591</v>
+        <v>585</v>
       </c>
     </row>
   </sheetData>
@@ -4994,8 +5050,8 @@
   </sheetPr>
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView topLeftCell="D20" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5038,35 +5094,35 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="B2" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="C2" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="H2" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="C3" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B4" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C4" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="E4" t="s">
         <v>55</v>
@@ -5077,339 +5133,345 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>346</v>
+      </c>
+      <c r="B5" t="s">
+        <v>347</v>
+      </c>
+      <c r="C5" t="s">
+        <v>348</v>
+      </c>
+      <c r="E5" t="s">
+        <v>349</v>
+      </c>
+      <c r="G5" t="s">
         <v>350</v>
-      </c>
-      <c r="B5" t="s">
-        <v>351</v>
-      </c>
-      <c r="C5" t="s">
-        <v>352</v>
-      </c>
-      <c r="E5" t="s">
-        <v>353</v>
-      </c>
-      <c r="G5" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C6" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="B7" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="C7" t="s">
-        <v>359</v>
+        <v>781</v>
       </c>
       <c r="D7" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="H7" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="B8" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="C8" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="B9" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="C9" t="s">
-        <v>367</v>
+        <v>362</v>
+      </c>
+      <c r="E9" t="s">
+        <v>767</v>
+      </c>
+      <c r="F9" t="s">
+        <v>768</v>
       </c>
       <c r="H9" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="B10" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="C10" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="H10" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="B11" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="C11" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="D11" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="E11" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F11" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="B12" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="C12" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="C13" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="E13" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="F13" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="G13" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="C14" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="B15" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="C15" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="B16" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="C16" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="D16" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="C17" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>391</v>
+      </c>
+      <c r="B18" t="s">
+        <v>392</v>
+      </c>
+      <c r="C18" t="s">
+        <v>393</v>
+      </c>
+      <c r="D18" t="s">
+        <v>394</v>
+      </c>
+      <c r="E18" t="s">
+        <v>395</v>
+      </c>
+      <c r="F18" t="s">
         <v>396</v>
       </c>
-      <c r="B18" t="s">
+      <c r="H18" t="s">
         <v>397</v>
-      </c>
-      <c r="C18" t="s">
-        <v>398</v>
-      </c>
-      <c r="D18" t="s">
-        <v>399</v>
-      </c>
-      <c r="E18" t="s">
-        <v>400</v>
-      </c>
-      <c r="F18" t="s">
-        <v>401</v>
-      </c>
-      <c r="H18" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>398</v>
+      </c>
+      <c r="B19" t="s">
+        <v>399</v>
+      </c>
+      <c r="C19" t="s">
+        <v>400</v>
+      </c>
+      <c r="D19" t="s">
+        <v>401</v>
+      </c>
+      <c r="E19" t="s">
+        <v>402</v>
+      </c>
+      <c r="F19" t="s">
         <v>403</v>
       </c>
-      <c r="B19" t="s">
+      <c r="H19" t="s">
         <v>404</v>
-      </c>
-      <c r="C19" t="s">
-        <v>405</v>
-      </c>
-      <c r="D19" t="s">
-        <v>406</v>
-      </c>
-      <c r="E19" t="s">
-        <v>407</v>
-      </c>
-      <c r="F19" t="s">
-        <v>408</v>
-      </c>
-      <c r="H19" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="B20" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="C20" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="D20" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="H20" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>410</v>
+      </c>
+      <c r="B21" t="s">
+        <v>411</v>
+      </c>
+      <c r="C21" t="s">
+        <v>412</v>
+      </c>
+      <c r="D21" t="s">
+        <v>413</v>
+      </c>
+      <c r="E21" t="s">
+        <v>414</v>
+      </c>
+      <c r="F21" t="s">
         <v>415</v>
-      </c>
-      <c r="B21" t="s">
-        <v>416</v>
-      </c>
-      <c r="C21" t="s">
-        <v>417</v>
-      </c>
-      <c r="D21" t="s">
-        <v>418</v>
-      </c>
-      <c r="E21" t="s">
-        <v>419</v>
-      </c>
-      <c r="F21" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="B22" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="C22" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="D22" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="B23" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="C23" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="B24" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="C24" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="D24" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="B25" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="C25" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>430</v>
+      </c>
+      <c r="B26" t="s">
+        <v>431</v>
+      </c>
+      <c r="C26" t="s">
+        <v>432</v>
+      </c>
+      <c r="D26" t="s">
+        <v>433</v>
+      </c>
+      <c r="E26" t="s">
+        <v>434</v>
+      </c>
+      <c r="F26" t="s">
         <v>435</v>
       </c>
-      <c r="B26" t="s">
+      <c r="G26" t="s">
         <v>436</v>
       </c>
-      <c r="C26" t="s">
+      <c r="H26" t="s">
         <v>437</v>
-      </c>
-      <c r="D26" t="s">
-        <v>438</v>
-      </c>
-      <c r="E26" t="s">
-        <v>439</v>
-      </c>
-      <c r="F26" t="s">
-        <v>440</v>
-      </c>
-      <c r="G26" t="s">
-        <v>441</v>
-      </c>
-      <c r="H26" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="B27" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="C27" t="s">
         <v>86</v>
@@ -5417,131 +5479,131 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="C28" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="E28" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="F28" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="C29" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="E29" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="F29" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="C30" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="E30" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="G30" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="C31" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C32" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>453</v>
+      </c>
+      <c r="B33" t="s">
+        <v>454</v>
+      </c>
+      <c r="C33" t="s">
+        <v>455</v>
+      </c>
+      <c r="D33" t="s">
+        <v>456</v>
+      </c>
+      <c r="E33" t="s">
+        <v>457</v>
+      </c>
+      <c r="H33" t="s">
         <v>458</v>
-      </c>
-      <c r="B33" t="s">
-        <v>459</v>
-      </c>
-      <c r="C33" t="s">
-        <v>460</v>
-      </c>
-      <c r="D33" t="s">
-        <v>461</v>
-      </c>
-      <c r="E33" t="s">
-        <v>462</v>
-      </c>
-      <c r="H33" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="B34" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="C34" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
     </row>
     <row r="35" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
     </row>
     <row r="36" spans="1:8" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
+        <v>465</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>468</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>469</v>
+      </c>
+      <c r="G36" s="4" t="s">
         <v>470</v>
       </c>
-      <c r="B36" s="6" t="s">
-        <v>471</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>472</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>473</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>474</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>475</v>
-      </c>
       <c r="H36" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>
@@ -5561,8 +5623,8 @@
   </sheetPr>
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5605,155 +5667,155 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C2" t="s">
+        <v>287</v>
+      </c>
+      <c r="D2" t="s">
         <v>288</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="C2" t="s">
-        <v>290</v>
-      </c>
-      <c r="D2" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B3" t="s">
+        <v>290</v>
+      </c>
+      <c r="C3" t="s">
+        <v>291</v>
+      </c>
+      <c r="D3" t="s">
         <v>292</v>
-      </c>
-      <c r="B3" t="s">
-        <v>293</v>
-      </c>
-      <c r="C3" t="s">
-        <v>294</v>
-      </c>
-      <c r="D3" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C4" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B5" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C5" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>299</v>
+      </c>
+      <c r="B6" t="s">
+        <v>300</v>
+      </c>
+      <c r="C6" t="s">
+        <v>301</v>
+      </c>
+      <c r="D6" t="s">
         <v>302</v>
       </c>
-      <c r="B6" t="s">
+      <c r="H6" t="s">
         <v>303</v>
-      </c>
-      <c r="C6" t="s">
-        <v>304</v>
-      </c>
-      <c r="D6" t="s">
-        <v>305</v>
-      </c>
-      <c r="H6" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B7" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C7" t="s">
-        <v>309</v>
+        <v>781</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B8" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C8" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="H8" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B9" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C9" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C10" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="E10" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="F10" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>317</v>
+      </c>
+      <c r="C11" t="s">
+        <v>318</v>
+      </c>
+      <c r="E11" t="s">
+        <v>319</v>
+      </c>
+      <c r="F11" t="s">
+        <v>320</v>
+      </c>
+      <c r="H11" t="s">
         <v>321</v>
-      </c>
-      <c r="C11" t="s">
-        <v>322</v>
-      </c>
-      <c r="E11" t="s">
-        <v>323</v>
-      </c>
-      <c r="F11" t="s">
-        <v>324</v>
-      </c>
-      <c r="H11" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C12" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="H12" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B13" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="C13" t="s">
         <v>31</v>
@@ -5764,41 +5826,41 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="C14" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="E14" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="F14" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C15" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -5810,7 +5872,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5851,13 +5915,13 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C2" t="s">
         <v>227</v>
-      </c>
-      <c r="B2" t="s">
-        <v>228</v>
-      </c>
-      <c r="C2" t="s">
-        <v>229</v>
       </c>
       <c r="D2" t="s">
         <v>28</v>
@@ -5865,203 +5929,203 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C3" t="s">
         <v>230</v>
-      </c>
-      <c r="B3" t="s">
-        <v>231</v>
-      </c>
-      <c r="C3" t="s">
-        <v>232</v>
       </c>
       <c r="D3" t="s">
         <v>77</v>
       </c>
       <c r="H3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>232</v>
+      </c>
+      <c r="B4" t="s">
+        <v>233</v>
+      </c>
+      <c r="C4" t="s">
         <v>234</v>
-      </c>
-      <c r="B4" t="s">
-        <v>235</v>
-      </c>
-      <c r="C4" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B5" t="s">
+        <v>236</v>
+      </c>
+      <c r="C5" t="s">
         <v>237</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>238</v>
       </c>
-      <c r="C5" t="s">
+      <c r="H5" t="s">
         <v>239</v>
-      </c>
-      <c r="D5" t="s">
-        <v>240</v>
-      </c>
-      <c r="H5" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>240</v>
+      </c>
+      <c r="B6" t="s">
+        <v>241</v>
+      </c>
+      <c r="C6" t="s">
         <v>242</v>
-      </c>
-      <c r="B6" t="s">
-        <v>243</v>
-      </c>
-      <c r="C6" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B7" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C7" t="s">
-        <v>247</v>
+        <v>781</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C8" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>247</v>
+      </c>
+      <c r="B9" t="s">
+        <v>248</v>
+      </c>
+      <c r="C9" t="s">
+        <v>249</v>
+      </c>
+      <c r="D9" t="s">
         <v>250</v>
-      </c>
-      <c r="B9" t="s">
-        <v>251</v>
-      </c>
-      <c r="C9" t="s">
-        <v>252</v>
-      </c>
-      <c r="D9" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>251</v>
+      </c>
+      <c r="B10" t="s">
+        <v>252</v>
+      </c>
+      <c r="C10" t="s">
+        <v>253</v>
+      </c>
+      <c r="D10" t="s">
         <v>254</v>
-      </c>
-      <c r="B10" t="s">
-        <v>255</v>
-      </c>
-      <c r="C10" t="s">
-        <v>256</v>
-      </c>
-      <c r="D10" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>255</v>
+      </c>
+      <c r="B11" t="s">
+        <v>256</v>
+      </c>
+      <c r="C11" t="s">
+        <v>257</v>
+      </c>
+      <c r="E11" t="s">
         <v>258</v>
       </c>
-      <c r="B11" t="s">
-        <v>259</v>
-      </c>
-      <c r="C11" t="s">
-        <v>260</v>
-      </c>
-      <c r="E11" t="s">
-        <v>261</v>
-      </c>
       <c r="F11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>259</v>
+      </c>
+      <c r="B12" t="s">
+        <v>260</v>
+      </c>
+      <c r="C12" t="s">
+        <v>261</v>
+      </c>
+      <c r="E12" t="s">
         <v>262</v>
       </c>
-      <c r="B12" t="s">
-        <v>263</v>
-      </c>
-      <c r="C12" t="s">
-        <v>264</v>
-      </c>
-      <c r="E12" t="s">
-        <v>265</v>
-      </c>
       <c r="F12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>263</v>
+      </c>
+      <c r="B13" t="s">
+        <v>264</v>
+      </c>
+      <c r="C13" t="s">
+        <v>265</v>
+      </c>
+      <c r="E13" t="s">
         <v>266</v>
       </c>
-      <c r="B13" t="s">
-        <v>267</v>
-      </c>
-      <c r="C13" t="s">
-        <v>268</v>
-      </c>
-      <c r="E13" t="s">
-        <v>269</v>
-      </c>
       <c r="F13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C14" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E14" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C15" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="E15" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>273</v>
+      </c>
+      <c r="B16" t="s">
+        <v>274</v>
+      </c>
+      <c r="C16" t="s">
+        <v>275</v>
+      </c>
+      <c r="D16" t="s">
         <v>276</v>
-      </c>
-      <c r="B16" t="s">
-        <v>277</v>
-      </c>
-      <c r="C16" t="s">
-        <v>278</v>
-      </c>
-      <c r="D16" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B17" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C17" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D17" t="s">
         <v>28</v>
@@ -6069,19 +6133,19 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>280</v>
+      </c>
+      <c r="B18" t="s">
+        <v>281</v>
+      </c>
+      <c r="C18" t="s">
+        <v>282</v>
+      </c>
+      <c r="D18" t="s">
         <v>283</v>
       </c>
-      <c r="B18" t="s">
+      <c r="H18" t="s">
         <v>284</v>
-      </c>
-      <c r="C18" t="s">
-        <v>285</v>
-      </c>
-      <c r="D18" t="s">
-        <v>286</v>
-      </c>
-      <c r="H18" t="s">
-        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -6093,8 +6157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6137,279 +6201,279 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" t="s">
         <v>154</v>
-      </c>
-      <c r="B2" t="s">
-        <v>155</v>
       </c>
       <c r="C2" t="s">
         <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" t="s">
         <v>157</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>158</v>
-      </c>
-      <c r="C3" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B4" t="s">
         <v>160</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>161</v>
-      </c>
-      <c r="C4" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" t="s">
         <v>163</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>164</v>
       </c>
-      <c r="C5" t="s">
+      <c r="H5" t="s">
         <v>165</v>
-      </c>
-      <c r="H5" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B6" t="s">
         <v>167</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>168</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>169</v>
-      </c>
-      <c r="D6" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C7" t="s">
-        <v>172</v>
+        <v>781</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C8" t="s">
+        <v>172</v>
+      </c>
+      <c r="D8" t="s">
         <v>173</v>
-      </c>
-      <c r="C8" t="s">
-        <v>174</v>
-      </c>
-      <c r="D8" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C10" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>178</v>
+      </c>
+      <c r="B11" t="s">
+        <v>179</v>
+      </c>
+      <c r="C11" t="s">
         <v>180</v>
-      </c>
-      <c r="B11" t="s">
-        <v>181</v>
-      </c>
-      <c r="C11" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>181</v>
+      </c>
+      <c r="B12" t="s">
+        <v>182</v>
+      </c>
+      <c r="C12" t="s">
         <v>183</v>
-      </c>
-      <c r="B12" t="s">
-        <v>184</v>
-      </c>
-      <c r="C12" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C13" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C14" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>188</v>
+      </c>
+      <c r="C15" t="s">
+        <v>189</v>
+      </c>
+      <c r="E15" t="s">
         <v>190</v>
       </c>
-      <c r="C15" t="s">
+      <c r="F15" t="s">
         <v>191</v>
-      </c>
-      <c r="E15" t="s">
-        <v>192</v>
-      </c>
-      <c r="F15" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>192</v>
+      </c>
+      <c r="C16" t="s">
+        <v>193</v>
+      </c>
+      <c r="E16" t="s">
         <v>194</v>
       </c>
-      <c r="C16" t="s">
+      <c r="F16" t="s">
         <v>195</v>
       </c>
-      <c r="E16" t="s">
+      <c r="H16" t="s">
         <v>196</v>
-      </c>
-      <c r="F16" t="s">
-        <v>197</v>
-      </c>
-      <c r="H16" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>197</v>
+      </c>
+      <c r="B17" t="s">
+        <v>198</v>
+      </c>
+      <c r="C17" t="s">
         <v>199</v>
       </c>
-      <c r="B17" t="s">
+      <c r="D17" t="s">
         <v>200</v>
       </c>
-      <c r="C17" t="s">
+      <c r="E17" t="s">
+        <v>190</v>
+      </c>
+      <c r="F17" t="s">
         <v>201</v>
-      </c>
-      <c r="D17" t="s">
-        <v>202</v>
-      </c>
-      <c r="E17" t="s">
-        <v>192</v>
-      </c>
-      <c r="F17" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C18" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C19" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>206</v>
+      </c>
+      <c r="B20" t="s">
+        <v>207</v>
+      </c>
+      <c r="C20" t="s">
         <v>208</v>
-      </c>
-      <c r="B20" t="s">
-        <v>209</v>
-      </c>
-      <c r="C20" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>209</v>
+      </c>
+      <c r="C21" t="s">
+        <v>210</v>
+      </c>
+      <c r="E21" t="s">
         <v>211</v>
       </c>
-      <c r="C21" t="s">
+      <c r="F21" t="s">
         <v>212</v>
-      </c>
-      <c r="E21" t="s">
-        <v>213</v>
-      </c>
-      <c r="F21" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>213</v>
+      </c>
+      <c r="B22" t="s">
+        <v>214</v>
+      </c>
+      <c r="C22" t="s">
         <v>215</v>
       </c>
-      <c r="B22" t="s">
+      <c r="D22" t="s">
         <v>216</v>
       </c>
-      <c r="C22" t="s">
+      <c r="E22" t="s">
+        <v>194</v>
+      </c>
+      <c r="F22" t="s">
         <v>217</v>
-      </c>
-      <c r="D22" t="s">
-        <v>218</v>
-      </c>
-      <c r="E22" t="s">
-        <v>196</v>
-      </c>
-      <c r="F22" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>218</v>
+      </c>
+      <c r="B23" t="s">
+        <v>219</v>
+      </c>
+      <c r="C23" t="s">
         <v>220</v>
       </c>
-      <c r="B23" t="s">
+      <c r="D23" t="s">
         <v>221</v>
-      </c>
-      <c r="C23" t="s">
-        <v>222</v>
-      </c>
-      <c r="D23" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>222</v>
+      </c>
+      <c r="C24" t="s">
+        <v>223</v>
+      </c>
+      <c r="E24" t="s">
         <v>224</v>
       </c>
-      <c r="C24" t="s">
-        <v>225</v>
-      </c>
-      <c r="E24" t="s">
-        <v>226</v>
-      </c>
       <c r="F24" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>